<commit_message>
Update premarket movers data
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PREMARKET_MOVERS.xlsx
+++ b/PREMARKET_MOVERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daqui\PycharmProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B009DBD-A08A-402E-8990-5169471DE8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030A1260-BE0D-44D4-A3BB-2E14C9059C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-2865" windowWidth="29040" windowHeight="15720" xr2:uid="{4ABA9207-3106-4195-AAA6-90B2EFAF49CB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{4ABA9207-3106-4195-AAA6-90B2EFAF49CB}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -51,269 +51,254 @@
     <t>Pre Market Top Losers</t>
   </si>
   <si>
-    <t>NEM</t>
-  </si>
-  <si>
-    <t>Newmont Goldcorp</t>
-  </si>
-  <si>
-    <t>NOC</t>
-  </si>
-  <si>
-    <t>Northrop Grumman</t>
-  </si>
-  <si>
-    <t>626.24+49.23+8.53%</t>
-  </si>
-  <si>
-    <t>HII</t>
-  </si>
-  <si>
-    <t>Huntington Ingalls.</t>
-  </si>
-  <si>
-    <t>379.63+23.18+6.50%</t>
-  </si>
-  <si>
-    <t>LMT</t>
-  </si>
-  <si>
-    <t>Lockheed Martin</t>
-  </si>
-  <si>
-    <t>535.30+38.43+7.73%</t>
-  </si>
-  <si>
-    <t>LHX</t>
-  </si>
-  <si>
-    <t>L3Harris Technolog.</t>
-  </si>
-  <si>
-    <t>333.02+23.26+7.51%</t>
-  </si>
-  <si>
-    <t>GD</t>
-  </si>
-  <si>
-    <t>General Dynamics</t>
-  </si>
-  <si>
-    <t>366.00+20.36+5.89%</t>
-  </si>
-  <si>
-    <t>RTX</t>
-  </si>
-  <si>
-    <t>Rtx Corp</t>
-  </si>
-  <si>
-    <t>193.24+7.51+4.04%</t>
-  </si>
-  <si>
-    <t>PLTR</t>
-  </si>
-  <si>
-    <t>Palantir</t>
-  </si>
-  <si>
-    <t>186.62+4.94+2.72%</t>
-  </si>
-  <si>
-    <t>HWM</t>
-  </si>
-  <si>
-    <t>Howmet</t>
-  </si>
-  <si>
-    <t>215.77+4.87+2.31%</t>
-  </si>
-  <si>
-    <t>AMTM</t>
-  </si>
-  <si>
-    <t>Amentum Holdings L.</t>
-  </si>
-  <si>
-    <t>31.91+0.72+2.31%</t>
-  </si>
-  <si>
-    <t>TDG</t>
-  </si>
-  <si>
-    <t>Transdigm</t>
-  </si>
-  <si>
-    <t>1,413.31+28.06+2.03%</t>
-  </si>
-  <si>
-    <t>TFX</t>
-  </si>
-  <si>
-    <t>Teleflex</t>
-  </si>
-  <si>
-    <t>119.93-6.60-5.22%</t>
-  </si>
-  <si>
-    <t>105.30-2.71-2.51%</t>
-  </si>
-  <si>
-    <t>CTVA</t>
-  </si>
-  <si>
-    <t>Corteva Inc</t>
-  </si>
-  <si>
-    <t>66.88-1.66-2.42%</t>
-  </si>
-  <si>
-    <t>HIG</t>
-  </si>
-  <si>
-    <t>Hartford</t>
-  </si>
-  <si>
-    <t>133.18-2.72-2.00%</t>
-  </si>
-  <si>
-    <t>PNR</t>
-  </si>
-  <si>
-    <t>Pentair PLC</t>
-  </si>
-  <si>
-    <t>98.50-1.56-1.56%</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Agilent Technologi.</t>
-  </si>
-  <si>
-    <t>145.64-2.17-1.47%</t>
-  </si>
-  <si>
-    <t>KKR</t>
-  </si>
-  <si>
-    <t>KKR &amp; Co LP</t>
-  </si>
-  <si>
-    <t>129.00-1.83-1.40%</t>
-  </si>
-  <si>
-    <t>DRI</t>
-  </si>
-  <si>
-    <t>Darden Restaurants</t>
-  </si>
-  <si>
-    <t>197.00-2.77-1.39%</t>
-  </si>
-  <si>
-    <t>APP</t>
-  </si>
-  <si>
-    <t>Applovin Corp</t>
-  </si>
-  <si>
-    <t>625.00-7.92-1.25%</t>
-  </si>
-  <si>
-    <t>INTU</t>
-  </si>
-  <si>
-    <t>Intuit Inc</t>
-  </si>
-  <si>
-    <t>640.88-10.27-1.58%</t>
-  </si>
-  <si>
-    <t>8.53%</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>6.50%</t>
-  </si>
-  <si>
-    <t>7.73%</t>
-  </si>
-  <si>
-    <t>7.51%</t>
-  </si>
-  <si>
-    <t>5.89%</t>
-  </si>
-  <si>
-    <t>4.04%</t>
-  </si>
-  <si>
-    <t>2.72%</t>
-  </si>
-  <si>
-    <t>2.31%</t>
-  </si>
-  <si>
-    <t>2.03%</t>
-  </si>
-  <si>
-    <t>-5.22%</t>
-  </si>
-  <si>
-    <t>-2.51%</t>
-  </si>
-  <si>
-    <t>-2.42%</t>
-  </si>
-  <si>
-    <t>-2.00%</t>
-  </si>
-  <si>
-    <t>-1.56%</t>
-  </si>
-  <si>
-    <t>-1.47%</t>
-  </si>
-  <si>
-    <t>-1.40%</t>
-  </si>
-  <si>
-    <t>-1.39%</t>
-  </si>
-  <si>
-    <t>-1.25%</t>
-  </si>
-  <si>
-    <t>-1.58%</t>
-  </si>
-  <si>
-    <t>Pre Mark Move</t>
-  </si>
-  <si>
-    <t>KTOS</t>
-  </si>
-  <si>
-    <t>GMED</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>APLD</t>
-  </si>
-  <si>
     <t>OSCR</t>
+  </si>
+  <si>
+    <t>VST</t>
+  </si>
+  <si>
+    <t>Vistra Energy Corp</t>
+  </si>
+  <si>
+    <t>173.01+22.41+14.88%</t>
+  </si>
+  <si>
+    <t>CEG</t>
+  </si>
+  <si>
+    <t>Constellation Ener.</t>
+  </si>
+  <si>
+    <t>338.40+15.86+4.92%</t>
+  </si>
+  <si>
+    <t>NRG</t>
+  </si>
+  <si>
+    <t>NRG Energy Inc</t>
+  </si>
+  <si>
+    <t>149.60+6.07+4.23%</t>
+  </si>
+  <si>
+    <t>LUV</t>
+  </si>
+  <si>
+    <t>Southwest Airlines</t>
+  </si>
+  <si>
+    <t>44.34+1.42+3.31%</t>
+  </si>
+  <si>
+    <t>CZR</t>
+  </si>
+  <si>
+    <t>Caesars</t>
+  </si>
+  <si>
+    <t>25.90+0.83+3.31%</t>
+  </si>
+  <si>
+    <t>LRCX</t>
+  </si>
+  <si>
+    <t>Lam Research Corp</t>
+  </si>
+  <si>
+    <t>206.50+5.54+2.76%</t>
+  </si>
+  <si>
+    <t>PSKY</t>
+  </si>
+  <si>
+    <t>Paramount Skydance</t>
+  </si>
+  <si>
+    <t>12.60+0.33+2.69%</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>Intel Corporation</t>
+  </si>
+  <si>
+    <t>42.15+1.04+2.53%</t>
+  </si>
+  <si>
+    <t>KLAC</t>
+  </si>
+  <si>
+    <t>KLA Corporation</t>
+  </si>
+  <si>
+    <t>1,358.30+33.70+2.54%</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>Applied Materials</t>
+  </si>
+  <si>
+    <t>288.71+7.07+2.51%</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>General Motors</t>
+  </si>
+  <si>
+    <t>83.46-1.67-1.96%</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>MetLife Inc</t>
+  </si>
+  <si>
+    <t>78.37-1.41-1.77%</t>
+  </si>
+  <si>
+    <t>VRSK</t>
+  </si>
+  <si>
+    <t>Verisk</t>
+  </si>
+  <si>
+    <t>219.00-3.85-1.73%</t>
+  </si>
+  <si>
+    <t>QCOM</t>
+  </si>
+  <si>
+    <t>Qualcomm</t>
+  </si>
+  <si>
+    <t>178.75-3.12-1.72%</t>
+  </si>
+  <si>
+    <t>ZBH</t>
+  </si>
+  <si>
+    <t>Zimmer Biomet</t>
+  </si>
+  <si>
+    <t>92.85-1.23-1.31%</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>General Mills Inc</t>
+  </si>
+  <si>
+    <t>43.41-0.51-1.16%</t>
+  </si>
+  <si>
+    <t>TECH</t>
+  </si>
+  <si>
+    <t>Bio-Techne Corp</t>
+  </si>
+  <si>
+    <t>63.85-0.73-1.13%</t>
+  </si>
+  <si>
+    <t>PPL</t>
+  </si>
+  <si>
+    <t>PPL Corporation</t>
+  </si>
+  <si>
+    <t>34.36-0.31-0.89%</t>
+  </si>
+  <si>
+    <t>VTRS</t>
+  </si>
+  <si>
+    <t>Viatris Inc</t>
+  </si>
+  <si>
+    <t>12.49-0.11-0.87%</t>
+  </si>
+  <si>
+    <t>STLD</t>
+  </si>
+  <si>
+    <t>170.67-1.49-0.87%</t>
+  </si>
+  <si>
+    <t>+2.51%</t>
+  </si>
+  <si>
+    <t>NVO</t>
+  </si>
+  <si>
+    <t>LCRX</t>
+  </si>
+  <si>
+    <t>DKNG</t>
+  </si>
+  <si>
+    <t>WULF</t>
+  </si>
+  <si>
+    <t>+14.88%</t>
+  </si>
+  <si>
+    <t>+4.92%</t>
+  </si>
+  <si>
+    <t>+4.23%</t>
+  </si>
+  <si>
+    <t>+3.31%</t>
+  </si>
+  <si>
+    <t>+2.76%</t>
+  </si>
+  <si>
+    <t>+2.69%</t>
+  </si>
+  <si>
+    <t>+2.53%</t>
+  </si>
+  <si>
+    <t>+2.54%</t>
+  </si>
+  <si>
+    <t>-1.96%</t>
+  </si>
+  <si>
+    <t>-1.77%</t>
+  </si>
+  <si>
+    <t>-1.73%</t>
+  </si>
+  <si>
+    <t>-1.72%</t>
+  </si>
+  <si>
+    <t>-1.31%</t>
+  </si>
+  <si>
+    <t>-1.16%</t>
+  </si>
+  <si>
+    <t>-1.13%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +308,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -347,19 +339,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -691,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D069423D-0355-451A-857D-DE110EB9EE38}">
-  <dimension ref="B4:D58"/>
+  <dimension ref="B4:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,32 +709,35 @@
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>84</v>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
@@ -745,15 +745,18 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
@@ -761,15 +764,18 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>15</v>
       </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
@@ -777,15 +783,18 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>18</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
@@ -793,15 +802,18 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>21</v>
       </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
@@ -809,15 +821,18 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>24</v>
       </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
@@ -825,15 +840,18 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>27</v>
       </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
@@ -841,15 +859,18 @@
         <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
@@ -857,63 +878,63 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>33</v>
       </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>0.12839999999999999</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2">
-        <v>7.3200000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
-        <v>7.0999999999999994E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2">
-        <v>6.3700000000000007E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2">
-        <v>6.1499999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
@@ -935,15 +956,12 @@
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D37" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>0</v>
       </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
     </row>
@@ -951,8 +969,11 @@
       <c r="B39" t="s">
         <v>36</v>
       </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
@@ -960,151 +981,121 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="D55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1114,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5523BC-9990-4E74-AAED-C2125B6405A8}">
-  <dimension ref="C5:E49"/>
+  <dimension ref="C5:E172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E49"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1147,18 +1138,14 @@
         <v>8</v>
       </c>
       <c r="E7" t="str">
-        <f>RIGHT(D7,5)</f>
-        <v>8.53%</v>
+        <f>RIGHT(D7,7)</f>
+        <v>+14.88%</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8:E29" si="0">RIGHT(D8,5)</f>
-        <v/>
-      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
@@ -1168,8 +1155,8 @@
         <v>11</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>6.50%</v>
+        <f>RIGHT(D9,6)</f>
+        <v>+4.92%</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.35">
@@ -1177,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E10:E25" si="0">RIGHT(D10,6)</f>
         <v/>
       </c>
     </row>
@@ -1190,7 +1177,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>7.73%</v>
+        <v>+4.23%</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.35">
@@ -1211,7 +1198,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>7.51%</v>
+        <v>+3.31%</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.35">
@@ -1232,7 +1219,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>5.89%</v>
+        <v>+3.31%</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.35">
@@ -1253,7 +1240,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>4.04%</v>
+        <v>+2.76%</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
@@ -1274,7 +1261,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>2.72%</v>
+        <v>+2.69%</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
@@ -1295,7 +1282,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>2.31%</v>
+        <v>+2.53%</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
@@ -1316,7 +1303,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>2.31%</v>
+        <v>+2.54%</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.35">
@@ -1337,248 +1324,358 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>2.03%</v>
+        <v>+2.51%</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.06</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>Price</v>
+        <v>67</v>
+      </c>
+      <c r="E29" s="6">
+        <v>2.6100000000000002E-2</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" t="str">
-        <f>RIGHT(D30,6)</f>
-        <v>-5.22%</v>
+        <v>68</v>
+      </c>
+      <c r="E30" s="6">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" ref="E31:E49" si="1">RIGHT(D31,6)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>-2.51%</v>
+        <v>69</v>
+      </c>
+      <c r="E31" s="6">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>40</v>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="1"/>
-        <v>-2.42%</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" ref="E35:E53" si="1">RIGHT(D35,6)</f>
+        <v>-1.96%</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>-2.00%</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.77%</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>-1.56%</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.73%</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>-1.47%</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="D41" t="s">
+        <v>47</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.72%</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>-1.40%</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.31%</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>-1.39%</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.16%</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>-1.25%</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-1.13%</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>-1.58%</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>-0.89%</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" t="s">
         <v>62</v>
       </c>
-      <c r="E49" t="str">
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>-0.87%</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>-0.87%</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2.6100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C59" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C60" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" s="4"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C146" s="5"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C148" s="3"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C150" s="5"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C152" s="3"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C154" s="5"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C156" s="3"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C158" s="5"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C160" s="3"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C162" s="5"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C164" s="3"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C168" s="3"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C172" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>